<commit_message>
update the webserice list
</commit_message>
<xml_diff>
--- a/Requirements/WebServiceList.xlsx
+++ b/Requirements/WebServiceList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="740" windowWidth="25600" windowHeight="14700" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>IPCS webservices</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>#</t>
+  </si>
+  <si>
+    <t>recommendation request,send email to school to recommend the service</t>
   </si>
 </sst>
 </file>
@@ -498,7 +501,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -649,9 +652,13 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3"/>
+    <row r="12" spans="1:6" ht="60">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -662,7 +669,6 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>